<commit_message>
2nd commit With the corrected form of the EXCEL
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d9ddf677702e2882/Desktop/sparta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_AD4DB114E441178AC67DF4952655EB28693EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{649D77DF-FAD6-405C-A467-F1309CC88FE0}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_AD4DB114E441178AC67DF4952655EB28693EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9D0E696-0C22-4FA9-A92A-F14FD9B01234}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Number</t>
+    <t>Grade</t>
   </si>
   <si>
-    <t>Grade</t>
+    <t>Student ID</t>
   </si>
 </sst>
 </file>
@@ -352,20 +352,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>4683</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1111</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>